<commit_message>
add spaceFilter to table
</commit_message>
<xml_diff>
--- a/heta/table.xlsx
+++ b/heta/table.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="namespaces" sheetId="3" r:id="rId1"/>
@@ -13,12 +13,12 @@
     <sheet name="export julia" sheetId="5" r:id="rId4"/>
     <sheet name="import" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17562" uniqueCount="4824">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17562" uniqueCount="4825">
   <si>
     <t>on</t>
   </si>
@@ -14490,12 +14490,15 @@
   </si>
   <si>
     <t>Julia</t>
+  </si>
+  <si>
+    <t>spaceFilter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -14598,7 +14601,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -14614,9 +14617,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -14654,9 +14657,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -14691,7 +14694,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -14726,7 +14729,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -25454,8 +25457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F959"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A955" workbookViewId="0">
-      <selection activeCell="D958" sqref="D958"/>
+    <sheetView topLeftCell="A808" workbookViewId="0">
+      <selection activeCell="H979" sqref="H979"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -42737,7 +42740,7 @@
   <dimension ref="A1:J959"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -42760,7 +42763,7 @@
         <v>4820</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>1</v>
+        <v>4824</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>15</v>
@@ -65719,8 +65722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E959"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -65740,7 +65743,7 @@
         <v>4820</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>1</v>
+        <v>4824</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>15</v>

</xml_diff>